<commit_message>
Adding Sockeye loss version and pre/postprocessing files
</commit_message>
<xml_diff>
--- a/Results/seq2seq_results.xlsx
+++ b/Results/seq2seq_results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/Documents/GitHub/sockeye-recipes/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{870D64CE-A399-994D-9916-D030C9E16D25}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E65D3B-9802-2F48-8828-FC2C0E4D5C01}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{63800894-6832-2440-9083-EFA27E428687}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -58,13 +58,28 @@
   </si>
   <si>
     <t>Beam Size</t>
+  </si>
+  <si>
+    <t>Original Newsela</t>
+  </si>
+  <si>
+    <t>Newela Version 2</t>
+  </si>
+  <si>
+    <t>Newsela Version 3</t>
+  </si>
+  <si>
+    <t>*Note that we changed our entity recognition to SpaCy's more fine-grained approach for v2 and v3</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,14 +96,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -233,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -245,16 +252,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -266,70 +303,124 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,204 +737,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3362A2F3-D871-0C4B-B155-B5D900831316}">
-  <dimension ref="B2:J9"/>
+  <dimension ref="B2:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:13">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="2:10" ht="34">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="14" t="s">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:13" ht="34">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="5" t="s">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="26">
+      <c r="E4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="22">
+      <c r="F4" s="16">
         <f>0.36379314092195*100</f>
         <v>36.379314092194996</v>
       </c>
-      <c r="F4" s="29">
+      <c r="G4" s="13">
         <f>100*0.589214253759426</f>
         <v>58.921425375942604</v>
       </c>
-      <c r="G4" s="30">
+      <c r="H4" s="14">
         <f>100*0.408176081534362</f>
         <v>40.817608153436204</v>
       </c>
-      <c r="H4" s="33">
+      <c r="I4" s="38">
         <f>100*0.268391861919164</f>
         <v>26.839186191916397</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="3">
+    <row r="5" spans="2:13">
+      <c r="B5" s="28"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="3">
         <v>5</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="16">
+      <c r="F5" s="17"/>
+      <c r="G5" s="7">
         <f>0.658387204449097*100</f>
         <v>65.838720444909711</v>
       </c>
-      <c r="G5" s="17">
+      <c r="H5" s="8">
         <f>0.424172286670437*100</f>
         <v>42.417228667043702</v>
       </c>
-      <c r="H5" s="17">
+      <c r="I5" s="8">
         <f>100*0.250024756307062</f>
         <v>25.002475630706201</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="25"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4">
+    <row r="6" spans="2:13">
+      <c r="B6" s="28"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="4">
         <v>10</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="27">
+      <c r="F6" s="18"/>
+      <c r="G6" s="9">
         <f>100*0.67706023296069</f>
         <v>67.706023296068992</v>
       </c>
-      <c r="G6" s="20">
+      <c r="H6" s="10">
         <f>100*0.426754534906805</f>
         <v>42.675453490680496</v>
       </c>
-      <c r="H6" s="19">
+      <c r="I6" s="10">
         <f>100*0.250360265440938</f>
         <v>25.036026544093797</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="25"/>
-      <c r="C7" s="25" t="s">
+    <row r="7" spans="2:13">
+      <c r="B7" s="28"/>
+      <c r="C7" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="21">
+      <c r="F7" s="17">
         <f>0.36379314092195*100</f>
         <v>36.379314092194996</v>
       </c>
-      <c r="F7" s="16">
+      <c r="G7" s="7">
         <f>100*0.591013402538371</f>
         <v>59.101340253837101</v>
       </c>
-      <c r="G7" s="17">
+      <c r="H7" s="8">
         <f>100*0.416572169336208</f>
         <v>41.657216933620802</v>
       </c>
-      <c r="H7" s="17">
+      <c r="I7" s="8">
         <f>100*0.265527587955381</f>
         <v>26.5527587955381</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="3">
+    <row r="8" spans="2:13">
+      <c r="B8" s="28"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="3">
         <v>5</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="16">
+      <c r="F8" s="17"/>
+      <c r="G8" s="7">
         <f>0.650766445514131*100</f>
         <v>65.076644551413096</v>
       </c>
-      <c r="G8" s="17">
+      <c r="H8" s="8">
         <f>0.424464303805217*100</f>
         <v>42.446430380521697</v>
       </c>
-      <c r="H8" s="32">
+      <c r="I8" s="15">
         <f>100*0.255230727840708</f>
         <v>25.523072784070798</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15" customHeight="1">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4">
+    <row r="9" spans="2:13" ht="15" customHeight="1">
+      <c r="B9" s="28"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="3">
         <v>10</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="18">
+      <c r="F9" s="17"/>
+      <c r="G9" s="7">
         <f>100*0.660247281857768</f>
         <v>66.024728185776809</v>
       </c>
-      <c r="G9" s="19">
+      <c r="H9" s="8">
         <f>100*0.425275529746539</f>
         <v>42.527552974653901</v>
       </c>
-      <c r="H9" s="31">
+      <c r="I9" s="41">
         <f>100*0.25472845577345</f>
         <v>25.472845577344998</v>
       </c>
     </row>
+    <row r="10" spans="2:13" ht="16" customHeight="1">
+      <c r="B10" s="28"/>
+      <c r="C10" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="50">
+        <v>1</v>
+      </c>
+      <c r="F10" s="54">
+        <f>100*0.358462182012152</f>
+        <v>35.846218201215201</v>
+      </c>
+      <c r="G10" s="47">
+        <f>100*0.633378912436381</f>
+        <v>63.337891243638097</v>
+      </c>
+      <c r="H10" s="52">
+        <f>100*0.411765673934286</f>
+        <v>41.176567393428599</v>
+      </c>
+      <c r="I10" s="48">
+        <f>100*0.340449469392756</f>
+        <v>34.044946939275597</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="39"/>
+      <c r="M10" s="60"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="28"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="51">
+        <v>5</v>
+      </c>
+      <c r="F11" s="55"/>
+      <c r="G11" s="61">
+        <f>100*0.695336409341215</f>
+        <v>69.533640934121493</v>
+      </c>
+      <c r="H11" s="49">
+        <f>100*0.431267677077956</f>
+        <v>43.126767707795601</v>
+      </c>
+      <c r="I11" s="49">
+        <f>100*0.340496168006096</f>
+        <v>34.049616800609598</v>
+      </c>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="60"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="28"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="51">
+        <v>10</v>
+      </c>
+      <c r="F12" s="55"/>
+      <c r="G12" s="46">
+        <f>100*0.709714023667025</f>
+        <v>70.971402366702492</v>
+      </c>
+      <c r="H12" s="53">
+        <f>100*0.430079493471261</f>
+        <v>43.0079493471261</v>
+      </c>
+      <c r="I12" s="49">
+        <f>100*0.340528178057137</f>
+        <v>34.052817805713701</v>
+      </c>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="60"/>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="28"/>
+      <c r="C13" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="50">
+        <v>1</v>
+      </c>
+      <c r="F13" s="54">
+        <f>100*0.358462182012152</f>
+        <v>35.846218201215201</v>
+      </c>
+      <c r="G13" s="47">
+        <f>100*0.604455940134864</f>
+        <v>60.445594013486406</v>
+      </c>
+      <c r="H13" s="52">
+        <f>100*0.407138925307856</f>
+        <v>40.7138925307856</v>
+      </c>
+      <c r="I13" s="57">
+        <f>100*0.340219418014607</f>
+        <v>34.021941801460699</v>
+      </c>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="60"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="28"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="51">
+        <v>5</v>
+      </c>
+      <c r="F14" s="55"/>
+      <c r="G14" s="45">
+        <f>100*0.671369116857777</f>
+        <v>67.136911685777704</v>
+      </c>
+      <c r="H14" s="53">
+        <f>100*0.422081610789433</f>
+        <v>42.208161078943299</v>
+      </c>
+      <c r="I14" s="58">
+        <f>100*0.340232752621877</f>
+        <v>34.023275262187703</v>
+      </c>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="60"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="29"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="42">
+        <v>10</v>
+      </c>
+      <c r="F15" s="56"/>
+      <c r="G15" s="43">
+        <f>100*0.688346930256841</f>
+        <v>68.834693025684103</v>
+      </c>
+      <c r="H15" s="44">
+        <f>100*0.421737032666688</f>
+        <v>42.173703266668802</v>
+      </c>
+      <c r="I15" s="59">
+        <f>100*0.340147808687311</f>
+        <v>34.014780868731101</v>
+      </c>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="60"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="32"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E2:G2"/>
+  <mergeCells count="20">
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="K10:L15"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B4:B15"/>
     <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F2:H2"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding in all model outputs
</commit_message>
<xml_diff>
--- a/Results/seq2seq_results.xlsx
+++ b/Results/seq2seq_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/Documents/GitHub/sockeye-recipes/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0EAE9C-0BC6-254F-9BF8-6A8048CBD9CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC6FD6C-A88A-8044-9A78-EB8C907A043B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="700" windowWidth="23800" windowHeight="16540" xr2:uid="{63800894-6832-2440-9083-EFA27E428687}"/>
+    <workbookView minimized="1" xWindow="2740" yWindow="540" windowWidth="23800" windowHeight="16540" xr2:uid="{63800894-6832-2440-9083-EFA27E428687}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -23,12 +23,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>Input_Format</t>
   </si>
@@ -198,10 +203,13 @@
     <t>Seq2Seq-LDCR</t>
   </si>
   <si>
-    <t>Newsela-V1</t>
-  </si>
-  <si>
     <t>Seq2Seq-R</t>
+  </si>
+  <si>
+    <t>Auto-Complex</t>
+  </si>
+  <si>
+    <t>Auto-Simple</t>
   </si>
 </sst>
 </file>
@@ -414,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,84 +586,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -674,6 +604,92 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -990,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764128D6-8239-9A43-B305-73DAA010AA3C}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1003,92 +1019,108 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="86" t="s">
-        <v>56</v>
+      <c r="C2" s="60" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="87">
+      <c r="C3" s="61">
         <f>100*0.363201298632058</f>
         <v>36.3201298632058</v>
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="87">
+      <c r="C4" s="61">
         <f>100*0.360304975885519</f>
         <v>36.030497588551903</v>
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="87">
+      <c r="C5" s="61">
         <f>100*0.359983168194613</f>
         <v>35.998316819461301</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="88">
+      <c r="C6" s="62">
         <f>100*0.343451991460067</f>
         <v>34.345199146006699</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="83" t="s">
+      <c r="B7" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="87">
+      <c r="C7" s="61">
         <f>100*0.360304975885519</f>
         <v>36.030497588551903</v>
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="87">
+      <c r="B8" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="61">
         <f>100*0.364725073208579</f>
         <v>36.4725073208579</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="89">
+      <c r="C9" s="63">
         <f>100*0.372244223768009</f>
         <v>37.224422376800895</v>
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="87">
+      <c r="C10" s="61">
         <f>100*0.353649187876813</f>
         <v>35.364918787681297</v>
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="90">
+      <c r="C11" s="64">
         <f>100*0.371089134818915</f>
         <v>37.108913481891499</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="65">
+        <v>27.72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="66">
+        <v>30.18</v>
       </c>
     </row>
   </sheetData>
@@ -1115,34 +1147,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:14">
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="71" t="s">
+      <c r="G2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="60" t="s">
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="72" t="s">
         <v>2</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="3:14" ht="34">
-      <c r="C3" s="59"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
       <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1152,24 +1184,24 @@
       <c r="I3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="61"/>
+      <c r="J3" s="73"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="3:14">
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="74" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="12">
         <v>1</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="80">
         <f>0.36379314092195*100</f>
         <v>36.379314092194996</v>
       </c>
@@ -1187,13 +1219,13 @@
       </c>
     </row>
     <row r="5" spans="3:14">
-      <c r="C5" s="66"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
       <c r="F5" s="3">
         <v>5</v>
       </c>
-      <c r="G5" s="69"/>
+      <c r="G5" s="81"/>
       <c r="H5" s="7">
         <f>0.650766445514131*100</f>
         <v>65.076644551413096</v>
@@ -1208,13 +1240,13 @@
       </c>
     </row>
     <row r="6" spans="3:14" ht="15" customHeight="1">
-      <c r="C6" s="67"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
       <c r="F6" s="4">
         <v>10</v>
       </c>
-      <c r="G6" s="70"/>
+      <c r="G6" s="82"/>
       <c r="H6" s="9">
         <f>100*0.660247281857768</f>
         <v>66.024728185776809</v>
@@ -1229,19 +1261,19 @@
       </c>
     </row>
     <row r="7" spans="3:14" ht="15" customHeight="1">
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="77" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="80">
         <f>0.36379314092195*100</f>
         <v>36.379314092194996</v>
       </c>
@@ -1259,13 +1291,13 @@
       </c>
     </row>
     <row r="8" spans="3:14" ht="15" customHeight="1">
-      <c r="C8" s="66"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="66"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="78"/>
       <c r="F8" s="3">
         <v>5</v>
       </c>
-      <c r="G8" s="69"/>
+      <c r="G8" s="81"/>
       <c r="H8" s="7">
         <f>100*0.6667034520998</f>
         <v>66.670345209979999</v>
@@ -1280,13 +1312,13 @@
       </c>
     </row>
     <row r="9" spans="3:14" ht="15" customHeight="1">
-      <c r="C9" s="67"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="67"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="79"/>
       <c r="F9" s="4">
         <v>10</v>
       </c>
-      <c r="G9" s="70"/>
+      <c r="G9" s="82"/>
       <c r="H9" s="46">
         <f>100*0.682087556614694</f>
         <v>68.208755661469397</v>
@@ -1655,19 +1687,19 @@
       <c r="N42" s="31"/>
     </row>
     <row r="43" spans="3:14">
-      <c r="C43" s="65" t="s">
+      <c r="C43" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="D43" s="62" t="s">
+      <c r="D43" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="62" t="s">
+      <c r="E43" s="74" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="24">
         <v>1</v>
       </c>
-      <c r="G43" s="76">
+      <c r="G43" s="88">
         <f>100*0.358462182012152</f>
         <v>35.846218201215201</v>
       </c>
@@ -1683,20 +1715,20 @@
         <f>100*0.340449469392756</f>
         <v>34.044946939275597</v>
       </c>
-      <c r="L43" s="57" t="s">
+      <c r="L43" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="M43" s="57"/>
+      <c r="M43" s="69"/>
       <c r="N43" s="31"/>
     </row>
     <row r="44" spans="3:14">
-      <c r="C44" s="66"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
+      <c r="C44" s="78"/>
+      <c r="D44" s="75"/>
+      <c r="E44" s="75"/>
       <c r="F44" s="25">
         <v>5</v>
       </c>
-      <c r="G44" s="77"/>
+      <c r="G44" s="89"/>
       <c r="H44" s="32">
         <f>100*0.695336409341215</f>
         <v>69.533640934121493</v>
@@ -1709,18 +1741,18 @@
         <f>100*0.340496168006096</f>
         <v>34.049616800609598</v>
       </c>
-      <c r="L44" s="57"/>
-      <c r="M44" s="57"/>
+      <c r="L44" s="69"/>
+      <c r="M44" s="69"/>
       <c r="N44" s="31"/>
     </row>
     <row r="45" spans="3:14">
-      <c r="C45" s="67"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
       <c r="F45" s="17">
         <v>10</v>
       </c>
-      <c r="G45" s="78"/>
+      <c r="G45" s="90"/>
       <c r="H45" s="45">
         <f>100*0.709714023667025</f>
         <v>70.971402366702492</v>
@@ -1733,24 +1765,24 @@
         <f>100*0.340528178057137</f>
         <v>34.052817805713701</v>
       </c>
-      <c r="L45" s="57"/>
-      <c r="M45" s="57"/>
+      <c r="L45" s="69"/>
+      <c r="M45" s="69"/>
       <c r="N45" s="31"/>
     </row>
     <row r="46" spans="3:14">
-      <c r="C46" s="65" t="s">
+      <c r="C46" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="79" t="s">
+      <c r="D46" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="E46" s="62" t="s">
+      <c r="E46" s="74" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="24">
         <v>1</v>
       </c>
-      <c r="G46" s="76">
+      <c r="G46" s="88">
         <f>100*0.358462182012152</f>
         <v>35.846218201215201</v>
       </c>
@@ -1766,18 +1798,18 @@
         <f>100*0.340755824765627</f>
         <v>34.075582476562701</v>
       </c>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
+      <c r="L46" s="69"/>
+      <c r="M46" s="69"/>
       <c r="N46" s="31"/>
     </row>
     <row r="47" spans="3:14">
-      <c r="C47" s="66"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="63"/>
+      <c r="C47" s="78"/>
+      <c r="D47" s="92"/>
+      <c r="E47" s="75"/>
       <c r="F47" s="25">
         <v>5</v>
       </c>
-      <c r="G47" s="77"/>
+      <c r="G47" s="89"/>
       <c r="H47" s="20">
         <f>100*0.694048395883354</f>
         <v>69.404839588335392</v>
@@ -1790,17 +1822,17 @@
         <f>100*0.340792224691425</f>
         <v>34.079222469142501</v>
       </c>
-      <c r="L47" s="57"/>
-      <c r="M47" s="57"/>
+      <c r="L47" s="69"/>
+      <c r="M47" s="69"/>
     </row>
     <row r="48" spans="3:14" ht="16" customHeight="1">
-      <c r="C48" s="67"/>
-      <c r="D48" s="81"/>
-      <c r="E48" s="64"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="76"/>
       <c r="F48" s="17">
         <v>10</v>
       </c>
-      <c r="G48" s="78"/>
+      <c r="G48" s="90"/>
       <c r="H48" s="42">
         <f>100*0.711065982382695</f>
         <v>71.106598238269498</v>
@@ -1813,8 +1845,8 @@
         <f>100*0.34078052386673</f>
         <v>34.078052386673001</v>
       </c>
-      <c r="L48" s="57"/>
-      <c r="M48" s="57"/>
+      <c r="L48" s="69"/>
+      <c r="M48" s="69"/>
     </row>
     <row r="50" spans="10:10">
       <c r="J50" s="55">
@@ -1863,34 +1895,34 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="2" spans="2:13">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74" t="s">
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="86" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:13" ht="68">
-      <c r="B3" s="59"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
       <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1900,24 +1932,24 @@
       <c r="H3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="82"/>
+      <c r="I3" s="94"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="74" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
       </c>
-      <c r="F4" s="68">
+      <c r="F4" s="80">
         <f>0.36379314092195*100</f>
         <v>36.379314092194996</v>
       </c>
@@ -1935,13 +1967,13 @@
       </c>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="66"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
       <c r="E5" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="69"/>
+      <c r="F5" s="81"/>
       <c r="G5" s="7">
         <f>0.658387204449097*100</f>
         <v>65.838720444909711</v>
@@ -1956,13 +1988,13 @@
       </c>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="66"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
       <c r="E6" s="4">
         <v>10</v>
       </c>
-      <c r="F6" s="70"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="9">
         <f>100*0.67706023296069</f>
         <v>67.706023296068992</v>
@@ -1977,19 +2009,19 @@
       </c>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="74" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="12">
         <v>1</v>
       </c>
-      <c r="F7" s="68">
+      <c r="F7" s="80">
         <f>0.36379314092195*100</f>
         <v>36.379314092194996</v>
       </c>
@@ -2007,13 +2039,13 @@
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="66"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
       <c r="E8" s="3">
         <v>5</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="81"/>
       <c r="G8" s="7">
         <f>0.650766445514131*100</f>
         <v>65.076644551413096</v>
@@ -2028,13 +2060,13 @@
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="67"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
       <c r="E9" s="4">
         <v>10</v>
       </c>
-      <c r="F9" s="70"/>
+      <c r="F9" s="82"/>
       <c r="G9" s="9">
         <f>100*0.660247281857768</f>
         <v>66.024728185776809</v>
@@ -2049,19 +2081,19 @@
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="77" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="80">
         <f>0.36379314092195*100</f>
         <v>36.379314092194996</v>
       </c>
@@ -2079,13 +2111,13 @@
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="B11" s="66"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="3">
         <v>5</v>
       </c>
-      <c r="F11" s="69"/>
+      <c r="F11" s="81"/>
       <c r="G11" s="7">
         <f>100*0.6667034520998</f>
         <v>66.670345209979999</v>
@@ -2100,13 +2132,13 @@
       </c>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="67"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="67"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="79"/>
       <c r="E12" s="4">
         <v>10</v>
       </c>
-      <c r="F12" s="70"/>
+      <c r="F12" s="82"/>
       <c r="G12" s="9">
         <f>100*0.682087556614694</f>
         <v>68.208755661469397</v>
@@ -2131,19 +2163,19 @@
       <c r="I13" s="40"/>
     </row>
     <row r="14" spans="2:13">
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="74" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="24">
         <v>1</v>
       </c>
-      <c r="F14" s="76">
+      <c r="F14" s="88">
         <f>100*0.358462182012152</f>
         <v>35.846218201215201</v>
       </c>
@@ -2159,20 +2191,20 @@
         <f>100*0.340449469392756</f>
         <v>34.044946939275597</v>
       </c>
-      <c r="K14" s="57" t="s">
+      <c r="K14" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="57"/>
+      <c r="L14" s="69"/>
       <c r="M14" s="31"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="66"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="75"/>
       <c r="E15" s="25">
         <v>5</v>
       </c>
-      <c r="F15" s="77"/>
+      <c r="F15" s="89"/>
       <c r="G15" s="32">
         <f>100*0.695336409341215</f>
         <v>69.533640934121493</v>
@@ -2185,18 +2217,18 @@
         <f>100*0.340496168006096</f>
         <v>34.049616800609598</v>
       </c>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
       <c r="M15" s="31"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="67"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="64"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="76"/>
       <c r="E16" s="17">
         <v>10</v>
       </c>
-      <c r="F16" s="78"/>
+      <c r="F16" s="90"/>
       <c r="G16" s="42">
         <f>100*0.709714023667025</f>
         <v>70.971402366702492</v>
@@ -2209,24 +2241,24 @@
         <f>100*0.340528178057137</f>
         <v>34.052817805713701</v>
       </c>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
       <c r="M16" s="31"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="74" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="76">
+      <c r="F17" s="88">
         <f>100*0.358462182012152</f>
         <v>35.846218201215201</v>
       </c>
@@ -2242,18 +2274,18 @@
         <f>100*0.340755824765627</f>
         <v>34.075582476562701</v>
       </c>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="69"/>
       <c r="M17" s="31"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="66"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="63"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="25">
         <v>5</v>
       </c>
-      <c r="F18" s="77"/>
+      <c r="F18" s="89"/>
       <c r="G18" s="20">
         <f>100*0.694048395883354</f>
         <v>69.404839588335392</v>
@@ -2266,18 +2298,18 @@
         <f>100*0.340792224691425</f>
         <v>34.079222469142501</v>
       </c>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
       <c r="M18" s="31"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="B19" s="67"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="64"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="76"/>
       <c r="E19" s="17">
         <v>10</v>
       </c>
-      <c r="F19" s="78"/>
+      <c r="F19" s="90"/>
       <c r="G19" s="18">
         <f>100*0.711065982382695</f>
         <v>71.106598238269498</v>
@@ -2290,8 +2322,8 @@
         <f>100*0.34078052386673</f>
         <v>34.078052386673001</v>
       </c>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
       <c r="M19" s="31"/>
     </row>
   </sheetData>

</xml_diff>